<commit_message>
update from office pc
</commit_message>
<xml_diff>
--- a/MavenProject/src/test/resources/excelFolder/TestSuite.xlsx
+++ b/MavenProject/src/test/resources/excelFolder/TestSuite.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <workbookPr defaultThemeVersion="124226" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView windowHeight="8010" windowWidth="14805" xWindow="240" yWindow="105"/>
   </bookViews>
   <sheets>
-    <sheet name="TestCaseList" sheetId="1" r:id="rId1"/>
-    <sheet name="TestData" sheetId="2" r:id="rId2"/>
+    <sheet name="TestCaseList" r:id="rId1" sheetId="1"/>
+    <sheet name="TestData" r:id="rId2" sheetId="2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="20">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -32,21 +32,12 @@
     <t>ExecuteResult</t>
   </si>
   <si>
-    <t>AddressManagement2</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
     <t>Data  1</t>
   </si>
   <si>
     <t>Data  2</t>
   </si>
   <si>
-    <t>ExecuteRusult</t>
-  </si>
-  <si>
     <t>HomeAddress</t>
   </si>
   <si>
@@ -57,13 +48,41 @@
   </si>
   <si>
     <t>OfficeAddressUpdate</t>
+  </si>
+  <si>
+    <t>RegisterAccount</t>
+  </si>
+  <si>
+    <t>SearchAndViewDetail</t>
+  </si>
+  <si>
+    <t>AddMultipleDressToCart</t>
+  </si>
+  <si>
+    <t>SearchFromMenuCategory</t>
+  </si>
+  <si>
+    <t>dress</t>
+  </si>
+  <si>
+    <t>testselenium30@gmail.com</t>
+  </si>
+  <si>
+    <t>testselenium31@gmail.com</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Fail</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -75,6 +94,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -118,27 +145,32 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="2">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="6">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium9" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -155,10 +187,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -193,7 +225,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -228,7 +260,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -316,7 +348,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -325,13 +357,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -341,7 +373,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -350,7 +382,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -359,7 +391,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -369,12 +401,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -405,7 +437,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -424,7 +456,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -436,18 +468,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="21.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -468,38 +500,76 @@
       <c r="B2" t="s">
         <v>3</v>
       </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22" style="3" customWidth="1"/>
-    <col min="2" max="3" width="13.42578125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="14" style="3" customWidth="1"/>
-    <col min="5" max="5" width="14.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" customWidth="true" style="3" width="22.0" collapsed="true"/>
+    <col min="2" max="4" customWidth="true" style="3" width="13.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" style="3" width="14.0" collapsed="true"/>
+    <col min="6" max="16384" style="3" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -507,46 +577,83 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row ht="30" r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>10</v>
-      </c>
+      <c r="C2" s="4"/>
       <c r="D2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="4"/>
-    </row>
-    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row ht="30" r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="4"/>
+      <c r="D3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row ht="45" r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="4"/>
+      <c r="B4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row ht="45" r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="D4"/>
+    <hyperlink r:id="rId2" ref="D5"/>
+  </hyperlinks>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>